<commit_message>
gallery some detail fix
</commit_message>
<xml_diff>
--- a/other/xinhu/yotubeVideos.xlsx
+++ b/other/xinhu/yotubeVideos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE217BB-657D-4951-9188-DF7B0005BFF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAC0839-2BE6-40E1-96AB-37D5CF5BD533}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -319,7 +319,7 @@
     <t>AtKE8IycOzo</t>
   </si>
   <si>
-    <t>新湖李弘仁老師專題報導杏壇芬芳奬得主～身心奉獻為教育</t>
+    <t>新湖李弘仁老師專題報導杏壇芬芳奬得主</t>
   </si>
 </sst>
 </file>
@@ -679,8 +679,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F45" sqref="A1:F45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>